<commit_message>
version before rice 3D model modification
</commit_message>
<xml_diff>
--- a/fspm-wheat/example/NEMA/Measured_Value/inputs/cnwheat/elements_inputs.xlsx
+++ b/fspm-wheat/example/NEMA/Measured_Value/inputs/cnwheat/elements_inputs.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="74">
   <si>
     <t>plant</t>
   </si>
@@ -279,6 +279,18 @@
   </si>
   <si>
     <t>axis total dry mass (g)</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>original Nstruct:mstruct</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>original mstruct:dry mass</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t xml:space="preserve">zhao note: refer to the given sample input data, the Nstruct:mstruct ratio is about 0.008, also considering N content in rice should typically higher than the wheat, the value 0.01 may be a proper value. </t>
     <phoneticPr fontId="18"/>
   </si>
 </sst>
@@ -481,7 +493,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="34">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -664,6 +676,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -992,7 +1010,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1075,6 +1093,12 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1237,7 +1261,13 @@
       <sheetName val="趙メモ"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0"/>
+      <sheetData sheetId="0">
+        <row r="5">
+          <cell r="G5">
+            <v>545</v>
+          </cell>
+        </row>
+      </sheetData>
       <sheetData sheetId="1"/>
       <sheetData sheetId="2"/>
       <sheetData sheetId="3">
@@ -1631,16 +1661,16 @@
   <dimension ref="A1:U77"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="F35" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="Q48" sqref="Q48"/>
+      <selection pane="bottomRight" activeCell="H4" sqref="H4:K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="14.625" customWidth="1"/>
-    <col min="3" max="3" width="18.125" customWidth="1"/>
+    <col min="3" max="3" width="10.875" customWidth="1"/>
     <col min="4" max="4" width="13.375" customWidth="1"/>
     <col min="5" max="5" width="25.25" customWidth="1"/>
     <col min="7" max="7" width="8.25" customWidth="1"/>
@@ -1844,74 +1874,74 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.4">
-      <c r="A4">
+    <row r="4" spans="1:21" s="28" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A4" s="28">
         <v>1</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="28" t="s">
         <v>21</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="28">
         <v>9</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="28" t="s">
         <v>25</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="F4">
-        <v>0</v>
-      </c>
-      <c r="G4">
-        <v>0</v>
-      </c>
-      <c r="H4">
+      <c r="F4" s="28">
+        <v>0</v>
+      </c>
+      <c r="G4" s="28">
+        <v>0</v>
+      </c>
+      <c r="H4" s="28">
         <f>($H$61*N4)/11</f>
         <v>6.6055610637861264</v>
       </c>
-      <c r="I4">
-        <f t="shared" ref="I4:I10" si="0">H4*10</f>
+      <c r="I4" s="28">
+        <f t="shared" ref="I4:I9" si="0">H4*10</f>
         <v>66.055610637861264</v>
       </c>
-      <c r="J4">
+      <c r="J4" s="28">
         <f>K4*$H$55</f>
         <v>2.3999999999999998E-3</v>
       </c>
-      <c r="K4">
+      <c r="K4" s="28">
         <f>C53</f>
         <v>0.08</v>
       </c>
-      <c r="L4">
-        <v>0</v>
-      </c>
-      <c r="M4">
+      <c r="L4" s="28">
+        <v>0</v>
+      </c>
+      <c r="M4" s="28">
         <f>$E$59*N4</f>
         <v>1600.2941845252403</v>
       </c>
-      <c r="N4" s="3">
+      <c r="N4" s="29">
         <f>[1]趙メモ!$P$18</f>
         <v>1.8679999999999999E-3</v>
       </c>
-      <c r="O4">
+      <c r="O4" s="28">
         <v>2.5</v>
       </c>
-      <c r="P4">
-        <v>0</v>
-      </c>
-      <c r="Q4">
-        <v>0</v>
-      </c>
-      <c r="R4">
-        <v>0</v>
-      </c>
-      <c r="S4">
+      <c r="P4" s="28">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="28">
+        <v>0</v>
+      </c>
+      <c r="R4" s="28">
+        <v>0</v>
+      </c>
+      <c r="S4" s="28">
         <v>18</v>
       </c>
-      <c r="T4" t="b">
-        <v>0</v>
-      </c>
-      <c r="U4">
+      <c r="T4" s="28" t="b">
+        <v>0</v>
+      </c>
+      <c r="U4" s="28">
         <v>0</v>
       </c>
     </row>
@@ -2057,74 +2087,74 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.4">
-      <c r="A7">
+    <row r="7" spans="1:21" s="28" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A7" s="28">
         <v>1</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="28" t="s">
         <v>21</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="28">
         <v>10</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="28" t="s">
         <v>25</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="F7">
-        <v>0</v>
-      </c>
-      <c r="G7">
-        <v>0</v>
-      </c>
-      <c r="H7">
+      <c r="F7" s="28">
+        <v>0</v>
+      </c>
+      <c r="G7" s="28">
+        <v>0</v>
+      </c>
+      <c r="H7" s="28">
         <f>($H$61*N7)/11</f>
         <v>8.5168596478206027</v>
       </c>
-      <c r="I7">
+      <c r="I7" s="28">
         <f t="shared" si="0"/>
         <v>85.168596478206027</v>
       </c>
-      <c r="J7">
+      <c r="J7" s="28">
         <f>K7*$H$55</f>
         <v>2.1351689999999997E-3</v>
       </c>
-      <c r="K7">
+      <c r="K7" s="28">
         <f>C55</f>
         <v>7.1172299999999994E-2</v>
       </c>
-      <c r="L7">
-        <v>0</v>
-      </c>
-      <c r="M7">
+      <c r="L7" s="28">
+        <v>0</v>
+      </c>
+      <c r="M7" s="28">
         <f>$E$59*N7</f>
         <v>2063.3343380241122</v>
       </c>
-      <c r="N7" s="3">
+      <c r="N7" s="29">
         <f>[1]趙メモ!$P$17</f>
         <v>2.4085000000000001E-3</v>
       </c>
-      <c r="O7">
+      <c r="O7" s="28">
         <v>3.5</v>
       </c>
-      <c r="P7">
-        <v>0</v>
-      </c>
-      <c r="Q7">
-        <v>0</v>
-      </c>
-      <c r="R7">
-        <v>0</v>
-      </c>
-      <c r="S7">
+      <c r="P7" s="28">
+        <v>0</v>
+      </c>
+      <c r="Q7" s="28">
+        <v>0</v>
+      </c>
+      <c r="R7" s="28">
+        <v>0</v>
+      </c>
+      <c r="S7" s="28">
         <v>18</v>
       </c>
-      <c r="T7" t="b">
-        <v>0</v>
-      </c>
-      <c r="U7">
+      <c r="T7" s="28" t="b">
+        <v>0</v>
+      </c>
+      <c r="U7" s="28">
         <v>0</v>
       </c>
     </row>
@@ -2270,74 +2300,74 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.4">
-      <c r="A10">
+    <row r="10" spans="1:21" s="28" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A10" s="28">
         <v>1</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="28" t="s">
         <v>21</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="28">
         <v>11</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="28" t="s">
         <v>25</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E10" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="F10">
-        <v>0</v>
-      </c>
-      <c r="G10">
-        <v>0</v>
-      </c>
-      <c r="H10">
+      <c r="F10" s="28">
+        <v>0</v>
+      </c>
+      <c r="G10" s="28">
+        <v>0</v>
+      </c>
+      <c r="H10" s="28">
         <f>($H$61*N10)/11</f>
         <v>11.375851146787994</v>
       </c>
-      <c r="I10">
-        <f t="shared" si="0"/>
+      <c r="I10" s="28">
+        <f>H10*10</f>
         <v>113.75851146787994</v>
       </c>
-      <c r="J10">
+      <c r="J10" s="28">
         <f>K10*$H$55</f>
         <v>4.5351689999999995E-3</v>
       </c>
-      <c r="K10">
+      <c r="K10" s="28">
         <f>K4+K7</f>
         <v>0.15117229999999998</v>
       </c>
-      <c r="L10">
-        <v>0</v>
-      </c>
-      <c r="M10">
+      <c r="L10" s="28">
+        <v>0</v>
+      </c>
+      <c r="M10" s="28">
         <f>$E$59*N10</f>
         <v>2755.9670190672905</v>
       </c>
-      <c r="N10" s="3">
+      <c r="N10" s="29">
         <f>[1]趙メモ!$P$16</f>
         <v>3.2170000000000002E-3</v>
       </c>
-      <c r="O10">
+      <c r="O10" s="28">
         <v>8</v>
       </c>
-      <c r="P10">
-        <v>0</v>
-      </c>
-      <c r="Q10">
-        <v>0</v>
-      </c>
-      <c r="R10">
-        <v>0</v>
-      </c>
-      <c r="S10">
+      <c r="P10" s="28">
+        <v>0</v>
+      </c>
+      <c r="Q10" s="28">
+        <v>0</v>
+      </c>
+      <c r="R10" s="28">
+        <v>0</v>
+      </c>
+      <c r="S10" s="28">
         <v>18</v>
       </c>
-      <c r="T10" t="b">
-        <v>0</v>
-      </c>
-      <c r="U10">
+      <c r="T10" s="28" t="b">
+        <v>0</v>
+      </c>
+      <c r="U10" s="28">
         <v>0</v>
       </c>
     </row>
@@ -2553,74 +2583,74 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.4">
-      <c r="A14">
+    <row r="14" spans="1:21" s="28" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A14" s="28">
         <v>1</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="28" t="s">
         <v>21</v>
       </c>
-      <c r="C14">
+      <c r="C14" s="28">
         <v>12</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D14" s="28" t="s">
         <v>25</v>
       </c>
-      <c r="E14" t="s">
+      <c r="E14" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="F14">
-        <v>0</v>
-      </c>
-      <c r="G14">
-        <v>0</v>
-      </c>
-      <c r="H14">
+      <c r="F14" s="28">
+        <v>0</v>
+      </c>
+      <c r="G14" s="28">
+        <v>0</v>
+      </c>
+      <c r="H14" s="28">
         <f>($H$61*N14)/11</f>
         <v>10.315000868878016</v>
       </c>
-      <c r="I14">
+      <c r="I14" s="28">
         <f>H14*10</f>
         <v>103.15000868878016</v>
       </c>
-      <c r="J14">
+      <c r="J14" s="28">
         <f>K14*$H$55</f>
         <v>6.6703379999999987E-3</v>
       </c>
-      <c r="K14">
+      <c r="K14" s="28">
         <f>K10+K7</f>
         <v>0.22234459999999998</v>
       </c>
-      <c r="L14">
-        <v>0</v>
-      </c>
-      <c r="M14">
+      <c r="L14" s="28">
+        <v>0</v>
+      </c>
+      <c r="M14" s="28">
         <f>$E$59*N14</f>
         <v>2498.9604583833657</v>
       </c>
-      <c r="N14" s="3">
+      <c r="N14" s="29">
         <f>[1]趙メモ!$P$15</f>
         <v>2.9170000000000003E-3</v>
       </c>
-      <c r="O14">
+      <c r="O14" s="28">
         <v>15</v>
       </c>
-      <c r="P14">
-        <v>0</v>
-      </c>
-      <c r="Q14">
-        <v>0</v>
-      </c>
-      <c r="R14">
-        <v>0</v>
-      </c>
-      <c r="S14">
+      <c r="P14" s="28">
+        <v>0</v>
+      </c>
+      <c r="Q14" s="28">
+        <v>0</v>
+      </c>
+      <c r="R14" s="28">
+        <v>0</v>
+      </c>
+      <c r="S14" s="28">
         <v>18</v>
       </c>
-      <c r="T14" t="b">
-        <v>0</v>
-      </c>
-      <c r="U14">
+      <c r="T14" s="28" t="b">
+        <v>0</v>
+      </c>
+      <c r="U14" s="28">
         <v>0</v>
       </c>
     </row>
@@ -3524,7 +3554,7 @@
         <v>46.460232142857137</v>
       </c>
     </row>
-    <row r="49" spans="1:14" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:15" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A49" s="10"/>
       <c r="B49" s="11"/>
       <c r="C49" s="11"/>
@@ -3538,12 +3568,12 @@
       <c r="K49" s="11"/>
       <c r="L49" s="12"/>
     </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="50" spans="1:15" x14ac:dyDescent="0.4">
       <c r="N50" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="51" spans="1:14" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:15" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A51" s="17" t="s">
         <v>31</v>
       </c>
@@ -3555,7 +3585,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="52" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A52" s="13" t="s">
         <v>32</v>
       </c>
@@ -3572,7 +3602,7 @@
       <c r="K52" s="6"/>
       <c r="L52" s="7"/>
     </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="53" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A53" s="14">
         <f>[2]CNデータ!$G$8*1000</f>
         <v>28157.160000000007</v>
@@ -3590,7 +3620,7 @@
       <c r="K53" s="5"/>
       <c r="L53" s="9"/>
     </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="54" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A54" s="8"/>
       <c r="B54" s="5"/>
       <c r="C54" s="5" t="s">
@@ -3607,8 +3637,11 @@
       <c r="J54" s="5"/>
       <c r="K54" s="5"/>
       <c r="L54" s="9"/>
-    </row>
-    <row r="55" spans="1:14" x14ac:dyDescent="0.4">
+      <c r="N54" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="55" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A55" s="1" t="s">
         <v>30</v>
       </c>
@@ -3631,8 +3664,14 @@
       <c r="J55" s="5"/>
       <c r="K55" s="5"/>
       <c r="L55" s="9"/>
-    </row>
-    <row r="56" spans="1:14" x14ac:dyDescent="0.4">
+      <c r="N55">
+        <v>0.03</v>
+      </c>
+      <c r="O55" s="3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="56" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A56" s="2">
         <f>[2]CNデータ!$C$8/5</f>
         <v>0.84960000000000002</v>
@@ -3657,7 +3696,7 @@
       <c r="K56" s="5"/>
       <c r="L56" s="9"/>
     </row>
-    <row r="57" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="57" spans="1:15" x14ac:dyDescent="0.4">
       <c r="B57" s="5"/>
       <c r="C57" s="5">
         <v>0.8</v>
@@ -3680,8 +3719,11 @@
       <c r="J57" s="5"/>
       <c r="K57" s="5"/>
       <c r="L57" s="9"/>
-    </row>
-    <row r="58" spans="1:14" x14ac:dyDescent="0.4">
+      <c r="N57" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="58" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A58" s="3" t="s">
         <v>38</v>
       </c>
@@ -3702,8 +3744,11 @@
       <c r="J58" s="5"/>
       <c r="K58" s="5"/>
       <c r="L58" s="9"/>
-    </row>
-    <row r="59" spans="1:14" x14ac:dyDescent="0.4">
+      <c r="N58">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="59" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A59" s="4">
         <f>A62*C62</f>
         <v>0.65586149999999999</v>
@@ -3722,7 +3767,7 @@
       </c>
       <c r="L59" s="9"/>
     </row>
-    <row r="60" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="60" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A60" s="5"/>
       <c r="B60" s="5"/>
       <c r="C60" s="5"/>
@@ -3738,7 +3783,7 @@
       <c r="K60" s="5"/>
       <c r="L60" s="9"/>
     </row>
-    <row r="61" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="61" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A61" s="14" t="s">
         <v>45</v>
       </c>
@@ -3759,7 +3804,7 @@
       <c r="K61" s="5"/>
       <c r="L61" s="9"/>
     </row>
-    <row r="62" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="62" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A62" s="14">
         <f>SUM(N4,N7,N10,N14)</f>
         <v>1.04105E-2</v>
@@ -3778,7 +3823,7 @@
       <c r="K62" s="5"/>
       <c r="L62" s="9"/>
     </row>
-    <row r="63" spans="1:14" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:15" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A63" s="11"/>
       <c r="B63" s="11"/>
       <c r="C63" s="11"/>

</xml_diff>

<commit_message>
fixed the green_area issue, forcing it not drop to 0 so that the element will not be skipped
</commit_message>
<xml_diff>
--- a/fspm-wheat/example/NEMA/Measured_Value/inputs/cnwheat/elements_inputs.xlsx
+++ b/fspm-wheat/example/NEMA/Measured_Value/inputs/cnwheat/elements_inputs.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gyoso.cho.TIRD\source\WheatFspm\WheatFspm\fspm-wheat\example\NEMA\Measured_Value\inputs\cnwheat\"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="68">
   <si>
     <t>plant</t>
   </si>
@@ -214,14 +214,6 @@
     <phoneticPr fontId="18"/>
   </si>
   <si>
-    <t>ear</t>
-    <phoneticPr fontId="18"/>
-  </si>
-  <si>
-    <t>1 culm dry mass (g)</t>
-    <phoneticPr fontId="18"/>
-  </si>
-  <si>
     <t>total C in whole plant (umol)</t>
     <phoneticPr fontId="18"/>
   </si>
@@ -258,26 +250,6 @@
     <phoneticPr fontId="18"/>
   </si>
   <si>
-    <t>C in grain (umol)</t>
-    <phoneticPr fontId="18"/>
-  </si>
-  <si>
-    <t>C in ear (umol)</t>
-    <phoneticPr fontId="18"/>
-  </si>
-  <si>
-    <t>dry mass in grain (g)</t>
-    <phoneticPr fontId="18"/>
-  </si>
-  <si>
-    <t>struct mass N(umol)</t>
-    <phoneticPr fontId="18"/>
-  </si>
-  <si>
-    <t>non-struct N (umol) in grain</t>
-    <phoneticPr fontId="18"/>
-  </si>
-  <si>
     <t>axis total dry mass (g)</t>
     <phoneticPr fontId="18"/>
   </si>
@@ -291,6 +263,10 @@
   </si>
   <si>
     <t xml:space="preserve">zhao note: refer to the given sample input data, the Nstruct:mstruct ratio is about 0.008, also considering N content in rice should typically higher than the wheat, the value 0.01 may be a proper value. </t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>t</t>
     <phoneticPr fontId="18"/>
   </si>
 </sst>
@@ -686,7 +662,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="18">
+  <borders count="20">
     <border>
       <left/>
       <right/>
@@ -881,6 +857,36 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -1010,7 +1016,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1099,6 +1105,27 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="14" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="14" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1157,6 +1184,1004 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="ja-JP"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="ja-JP"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>elements_inputs!$S$30:$X$30</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>2.6849999999999999E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.9581999999999981E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.9004E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.3575999999999998E-3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.4460000000000003E-4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4.77999999999998E-5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-B561-48B2-89DB-AFBB4DBF06E8}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>elements_inputs!$S$31:$X$31</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>3.1438E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.9265999999999997E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.9917999999999997E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-B561-48B2-89DB-AFBB4DBF06E8}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>elements_inputs!$S$32:$X$32</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>2.7525999999999996E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.0139999999999997E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-B561-48B2-89DB-AFBB4DBF06E8}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>elements_inputs!$S$33:$X$33</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1.4895999999999998E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.5459999999999998E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-B561-48B2-89DB-AFBB4DBF06E8}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="1821060143"/>
+        <c:axId val="1691776703"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1821060143"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ja-JP"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1691776703"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1691776703"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ja-JP"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1821060143"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="ja-JP"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="ja-JP"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1248,6 +2273,36 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>247650</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>238125</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="7" name="グラフ 6"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -1255,75 +2310,166 @@
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
-      <sheetName val="Sheet1"/>
-      <sheetName val="0803_生育調査"/>
-      <sheetName val="0726_生育調査"/>
-      <sheetName val="趙メモ"/>
+      <sheetName val="20240410_趙入力"/>
+      <sheetName val="Sheet2"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0">
+        <row r="4">
+          <cell r="AA4">
+            <v>8.7360000000000007E-2</v>
+          </cell>
+        </row>
         <row r="5">
-          <cell r="G5">
-            <v>545</v>
+          <cell r="AA5">
+            <v>0.12272000000000001</v>
+          </cell>
+        </row>
+        <row r="6">
+          <cell r="AA6">
+            <v>0.11232</v>
+          </cell>
+        </row>
+        <row r="7">
+          <cell r="AA7">
+            <v>5.6160000000000002E-2</v>
+          </cell>
+        </row>
+        <row r="9">
+          <cell r="Z9">
+            <v>0.65780000000000005</v>
+          </cell>
+        </row>
+        <row r="10">
+          <cell r="AA10">
+            <v>0.15344000000000002</v>
+          </cell>
+        </row>
+        <row r="11">
+          <cell r="AA11">
+            <v>0.10204000000000001</v>
+          </cell>
+        </row>
+        <row r="12">
+          <cell r="AA12">
+            <v>0.13156000000000001</v>
+          </cell>
+        </row>
+        <row r="15">
+          <cell r="AB15">
+            <v>777.13999999999942</v>
+          </cell>
+          <cell r="AC15">
+            <v>1.9219200000000002E-4</v>
+          </cell>
+          <cell r="AE15">
+            <v>284.23199999999997</v>
+          </cell>
+        </row>
+        <row r="16">
+          <cell r="AB16">
+            <v>1009.8833333333332</v>
+          </cell>
+          <cell r="AC16">
+            <v>2.6998400000000002E-4</v>
+          </cell>
+          <cell r="AE16">
+            <v>312.71685714285712</v>
+          </cell>
+        </row>
+        <row r="17">
+          <cell r="AB17">
+            <v>788.57999999999993</v>
+          </cell>
+          <cell r="AC17">
+            <v>2.47104E-4</v>
+          </cell>
+          <cell r="AE17">
+            <v>296.24399999999991</v>
+          </cell>
+        </row>
+        <row r="18">
+          <cell r="AB18">
+            <v>374.98500000000058</v>
+          </cell>
+          <cell r="AC18">
+            <v>1.23552E-4</v>
+          </cell>
+          <cell r="AE18">
+            <v>120.042</v>
+          </cell>
+        </row>
+        <row r="19">
+          <cell r="X19">
+            <v>17916.523333333331</v>
+          </cell>
+          <cell r="Y19">
+            <v>368.07285714285717</v>
+          </cell>
+        </row>
+        <row r="20">
+          <cell r="X20">
+            <v>23280.638333333332</v>
+          </cell>
+          <cell r="Y20">
+            <v>408.77571428571429</v>
+          </cell>
+        </row>
+        <row r="21">
+          <cell r="AB21">
+            <v>1.5983333333324481</v>
+          </cell>
+          <cell r="AC21">
+            <v>3.3756800000000006E-4</v>
+          </cell>
+          <cell r="AE21">
+            <v>277.28800000000001</v>
+          </cell>
+        </row>
+        <row r="22">
+          <cell r="AB22">
+            <v>996.29291666666631</v>
+          </cell>
+          <cell r="AC22">
+            <v>2.89432E-4</v>
+          </cell>
+          <cell r="AE22">
+            <v>81.520214285714289</v>
+          </cell>
+        </row>
+        <row r="23">
+          <cell r="AB23">
+            <v>737.66416666666555</v>
+          </cell>
+          <cell r="AC23">
+            <v>2.2448800000000001E-4</v>
+          </cell>
+          <cell r="AE23">
+            <v>75.983357142857145</v>
+          </cell>
+        </row>
+        <row r="35">
+          <cell r="H35">
+            <v>2.6849999999999999E-3</v>
+          </cell>
+        </row>
+        <row r="36">
+          <cell r="H36">
+            <v>3.1438E-3</v>
+          </cell>
+        </row>
+        <row r="37">
+          <cell r="H37">
+            <v>2.7525999999999996E-3</v>
+          </cell>
+        </row>
+        <row r="38">
+          <cell r="H38">
+            <v>1.4895999999999998E-3</v>
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3">
-        <row r="15">
-          <cell r="P15">
-            <v>2.9170000000000003E-3</v>
-          </cell>
-        </row>
-        <row r="16">
-          <cell r="P16">
-            <v>3.2170000000000002E-3</v>
-          </cell>
-        </row>
-        <row r="17">
-          <cell r="P17">
-            <v>2.4085000000000001E-3</v>
-          </cell>
-        </row>
-        <row r="18">
-          <cell r="P18">
-            <v>1.8679999999999999E-3</v>
-          </cell>
-        </row>
-        <row r="32">
-          <cell r="F32">
-            <v>2.400490943865E-3</v>
-          </cell>
-          <cell r="K32">
-            <v>2.8714156821000006E-3</v>
-          </cell>
-        </row>
-        <row r="33">
-          <cell r="F33">
-            <v>2.3800705916400002E-3</v>
-          </cell>
-          <cell r="K33">
-            <v>3.1450484019150001E-3</v>
-          </cell>
-        </row>
-        <row r="34">
-          <cell r="F34">
-            <v>2.1535617615750001E-3</v>
-          </cell>
-          <cell r="K34">
-            <v>4.655840307300001E-3</v>
-          </cell>
-        </row>
-        <row r="35">
-          <cell r="F35">
-            <v>8.9598222378000009E-4</v>
-          </cell>
-          <cell r="K35">
-            <v>4.4406412107750003E-3</v>
-          </cell>
-        </row>
-      </sheetData>
+      <sheetData sheetId="1" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -1355,34 +2501,6 @@
         <row r="9">
           <cell r="C9">
             <v>5.181</v>
-          </cell>
-          <cell r="G9">
-            <v>30.75787</v>
-          </cell>
-          <cell r="J9">
-            <v>0.44408571428571431</v>
-          </cell>
-        </row>
-        <row r="10">
-          <cell r="C10">
-            <v>3.4950000000000001</v>
-          </cell>
-          <cell r="G10">
-            <v>22.723325000000003</v>
-          </cell>
-          <cell r="J10">
-            <v>0.37446428571428569</v>
-          </cell>
-        </row>
-        <row r="11">
-          <cell r="C11">
-            <v>2.21</v>
-          </cell>
-          <cell r="G11">
-            <v>15.212166666666665</v>
-          </cell>
-          <cell r="J11">
-            <v>0.35044285714285717</v>
           </cell>
         </row>
       </sheetData>
@@ -1658,13 +2776,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U77"/>
+  <sheetPr codeName="Sheet1"/>
+  <dimension ref="A1:AI76"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H4" sqref="H4:K17"/>
+      <selection pane="bottomRight" activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -1674,9 +2793,14 @@
     <col min="4" max="4" width="13.375" customWidth="1"/>
     <col min="5" max="5" width="25.25" customWidth="1"/>
     <col min="7" max="7" width="8.25" customWidth="1"/>
-    <col min="12" max="12" width="13.375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.75" bestFit="1" customWidth="1"/>
+    <col min="8" max="10" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="7.25" customWidth="1"/>
+    <col min="13" max="13" width="10.875" customWidth="1"/>
+    <col min="14" max="14" width="14" customWidth="1"/>
+    <col min="18" max="18" width="10.875" customWidth="1"/>
+    <col min="19" max="19" width="8.5" customWidth="1"/>
+    <col min="23" max="23" width="9" customWidth="1"/>
+    <col min="24" max="24" width="12" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.4">
@@ -1896,32 +3020,32 @@
       <c r="G4" s="28">
         <v>0</v>
       </c>
-      <c r="H4" s="28">
-        <f>($H$61*N4)/11</f>
-        <v>6.6055610637861264</v>
-      </c>
-      <c r="I4" s="28">
+      <c r="H4" s="32">
+        <f>'[1]20240410_趙入力'!$AE$18/11</f>
+        <v>10.912909090909091</v>
+      </c>
+      <c r="I4" s="29">
         <f t="shared" ref="I4:I9" si="0">H4*10</f>
-        <v>66.055610637861264</v>
-      </c>
-      <c r="J4" s="28">
-        <f>K4*$H$55</f>
-        <v>2.3999999999999998E-3</v>
-      </c>
-      <c r="K4" s="28">
-        <f>C53</f>
-        <v>0.08</v>
+        <v>109.12909090909091</v>
+      </c>
+      <c r="J4" s="32">
+        <f>'[1]20240410_趙入力'!$AC$18</f>
+        <v>1.23552E-4</v>
+      </c>
+      <c r="K4" s="29">
+        <f>'[1]20240410_趙入力'!$AA$7</f>
+        <v>5.6160000000000002E-2</v>
       </c>
       <c r="L4" s="28">
         <v>0</v>
       </c>
-      <c r="M4" s="28">
-        <f>$E$59*N4</f>
-        <v>1600.2941845252403</v>
-      </c>
-      <c r="N4" s="29">
-        <f>[1]趙メモ!$P$18</f>
-        <v>1.8679999999999999E-3</v>
+      <c r="M4" s="32">
+        <f>'[1]20240410_趙入力'!$AB$18</f>
+        <v>374.98500000000058</v>
+      </c>
+      <c r="N4" s="32">
+        <f>'[1]20240410_趙入力'!$H$38</f>
+        <v>1.4895999999999998E-3</v>
       </c>
       <c r="O4" s="28">
         <v>2.5</v>
@@ -1967,32 +3091,31 @@
       <c r="G5">
         <v>0</v>
       </c>
-      <c r="H5">
-        <f>$H$47*N5/11</f>
-        <v>0.81515491535827256</v>
-      </c>
-      <c r="I5">
+      <c r="H5" s="34">
+        <f>'[1]20240410_趙入力'!$AE$22/11</f>
+        <v>7.4109285714285713</v>
+      </c>
+      <c r="I5" s="3">
         <f t="shared" si="0"/>
-        <v>8.1515491535827262</v>
-      </c>
-      <c r="J5">
-        <f>K5*$H$41</f>
-        <v>3.9992537313432837E-4</v>
-      </c>
-      <c r="K5">
-        <f>$C$47*N5</f>
-        <v>3.9992537313432837E-2</v>
+        <v>74.109285714285718</v>
+      </c>
+      <c r="J5" s="34">
+        <f>'[1]20240410_趙入力'!$AC$22</f>
+        <v>2.89432E-4</v>
+      </c>
+      <c r="K5" s="34">
+        <f>'[1]20240410_趙入力'!$AA$12</f>
+        <v>0.13156000000000001</v>
       </c>
       <c r="L5">
         <v>0</v>
       </c>
-      <c r="M5">
-        <f>$E$45*N5</f>
-        <v>199.61820149253748</v>
-      </c>
-      <c r="N5" s="3">
-        <f>[1]趙メモ!$F$35</f>
-        <v>8.9598222378000009E-4</v>
+      <c r="M5" s="34">
+        <f>'[1]20240410_趙入力'!$AB$22</f>
+        <v>996.29291666666631</v>
+      </c>
+      <c r="N5">
+        <v>1E-4</v>
       </c>
       <c r="O5">
         <v>0.1</v>
@@ -2038,32 +3161,31 @@
       <c r="G6">
         <v>0</v>
       </c>
-      <c r="H6">
-        <f>N6*$H$75/11</f>
-        <v>0.74139678893633654</v>
-      </c>
-      <c r="I6">
+      <c r="H6" s="34">
+        <f>'[1]20240410_趙入力'!$AE$23/11</f>
+        <v>6.9075779220779223</v>
+      </c>
+      <c r="I6" s="3">
         <f t="shared" si="0"/>
-        <v>7.4139678893633656</v>
-      </c>
-      <c r="J6">
-        <f>K6*$H$69</f>
-        <v>1.7126265824429386E-3</v>
-      </c>
-      <c r="K6">
-        <f>$C$75*N6</f>
-        <v>0.20551518989315262</v>
+        <v>69.075779220779225</v>
+      </c>
+      <c r="J6" s="34">
+        <f>'[1]20240410_趙入力'!$AC$23</f>
+        <v>2.2448800000000001E-4</v>
+      </c>
+      <c r="K6" s="3">
+        <f>'[1]20240410_趙入力'!$AA$11</f>
+        <v>0.10204000000000001</v>
       </c>
       <c r="L6">
         <v>0</v>
       </c>
-      <c r="M6">
-        <f>$E$73*N6</f>
-        <v>1502.0369434166209</v>
-      </c>
-      <c r="N6" s="3">
-        <f>[1]趙メモ!$K$35</f>
-        <v>4.4406412107750003E-3</v>
+      <c r="M6" s="34">
+        <f>'[1]20240410_趙入力'!$AB$23</f>
+        <v>737.66416666666555</v>
+      </c>
+      <c r="N6">
+        <v>2.0000000000000001E-4</v>
       </c>
       <c r="O6">
         <v>0.15</v>
@@ -2109,32 +3231,32 @@
       <c r="G7" s="28">
         <v>0</v>
       </c>
-      <c r="H7" s="28">
-        <f>($H$61*N7)/11</f>
-        <v>8.5168596478206027</v>
-      </c>
-      <c r="I7" s="28">
+      <c r="H7" s="32">
+        <f>'[1]20240410_趙入力'!$AE$17/11</f>
+        <v>26.93127272727272</v>
+      </c>
+      <c r="I7" s="29">
         <f t="shared" si="0"/>
-        <v>85.168596478206027</v>
-      </c>
-      <c r="J7" s="28">
-        <f>K7*$H$55</f>
-        <v>2.1351689999999997E-3</v>
-      </c>
-      <c r="K7" s="28">
-        <f>C55</f>
-        <v>7.1172299999999994E-2</v>
+        <v>269.31272727272722</v>
+      </c>
+      <c r="J7" s="32">
+        <f>'[1]20240410_趙入力'!$AC$17</f>
+        <v>2.47104E-4</v>
+      </c>
+      <c r="K7" s="29">
+        <f>'[1]20240410_趙入力'!$AA$6</f>
+        <v>0.11232</v>
       </c>
       <c r="L7" s="28">
         <v>0</v>
       </c>
-      <c r="M7" s="28">
-        <f>$E$59*N7</f>
-        <v>2063.3343380241122</v>
-      </c>
-      <c r="N7" s="29">
-        <f>[1]趙メモ!$P$17</f>
-        <v>2.4085000000000001E-3</v>
+      <c r="M7" s="32">
+        <f>'[1]20240410_趙入力'!$AB$17</f>
+        <v>788.57999999999993</v>
+      </c>
+      <c r="N7" s="32">
+        <f>'[1]20240410_趙入力'!$H$37</f>
+        <v>2.7525999999999996E-3</v>
       </c>
       <c r="O7" s="28">
         <v>3.5</v>
@@ -2180,32 +3302,31 @@
       <c r="G8">
         <v>0</v>
       </c>
-      <c r="H8">
-        <f>$H$47*N8/11</f>
-        <v>1.9592871475389053</v>
-      </c>
-      <c r="I8">
+      <c r="H8" s="34">
+        <f>'[1]20240410_趙入力'!$AE$22/11</f>
+        <v>7.4109285714285713</v>
+      </c>
+      <c r="I8" s="3">
         <f t="shared" si="0"/>
-        <v>19.592871475389053</v>
-      </c>
-      <c r="J8">
-        <f>K8*$H$41</f>
-        <v>9.6125120365912384E-4</v>
-      </c>
-      <c r="K8">
-        <f>$C$47*N8</f>
-        <v>9.6125120365912378E-2</v>
+        <v>74.109285714285718</v>
+      </c>
+      <c r="J8" s="34">
+        <f>'[1]20240410_趙入力'!$AC$22</f>
+        <v>2.89432E-4</v>
+      </c>
+      <c r="K8" s="34">
+        <f>'[1]20240410_趙入力'!$AA$12</f>
+        <v>0.13156000000000001</v>
       </c>
       <c r="L8">
         <v>0</v>
       </c>
-      <c r="M8">
-        <f>$E$45*N8</f>
-        <v>479.79760562108851</v>
-      </c>
-      <c r="N8" s="3">
-        <f>[1]趙メモ!$F$34</f>
-        <v>2.1535617615750001E-3</v>
+      <c r="M8" s="34">
+        <f>'[1]20240410_趙入力'!$AB$22</f>
+        <v>996.29291666666631</v>
+      </c>
+      <c r="N8">
+        <v>2.5000000000000001E-4</v>
       </c>
       <c r="O8">
         <v>0.1</v>
@@ -2251,32 +3372,31 @@
       <c r="G9">
         <v>0</v>
       </c>
-      <c r="H9">
-        <f>N9*$H$75/11</f>
-        <v>0.7773258162035025</v>
-      </c>
-      <c r="I9">
+      <c r="H9" s="34">
+        <f>'[1]20240410_趙入力'!$AE$23/11</f>
+        <v>6.9075779220779223</v>
+      </c>
+      <c r="I9" s="3">
         <f t="shared" si="0"/>
-        <v>7.7732581620350247</v>
-      </c>
-      <c r="J9">
-        <f>K9*$H$69</f>
-        <v>1.795622635430092E-3</v>
-      </c>
-      <c r="K9">
-        <f>$C$75*N9</f>
-        <v>0.21547471625161105</v>
+        <v>69.075779220779225</v>
+      </c>
+      <c r="J9" s="34">
+        <f>'[1]20240410_趙入力'!$AC$23</f>
+        <v>2.2448800000000001E-4</v>
+      </c>
+      <c r="K9" s="3">
+        <f>'[1]20240410_趙入力'!$AA$11</f>
+        <v>0.10204000000000001</v>
       </c>
       <c r="L9">
         <v>0</v>
       </c>
-      <c r="M9">
-        <f>$E$73*N9</f>
-        <v>1574.8275558142429</v>
-      </c>
-      <c r="N9" s="3">
-        <f>[1]趙メモ!$K$34</f>
-        <v>4.655840307300001E-3</v>
+      <c r="M9" s="34">
+        <f>'[1]20240410_趙入力'!$AB$23</f>
+        <v>737.66416666666555</v>
+      </c>
+      <c r="N9">
+        <v>4.0000000000000002E-4</v>
       </c>
       <c r="O9">
         <v>0.15</v>
@@ -2322,32 +3442,32 @@
       <c r="G10" s="28">
         <v>0</v>
       </c>
-      <c r="H10" s="28">
-        <f>($H$61*N10)/11</f>
-        <v>11.375851146787994</v>
-      </c>
-      <c r="I10" s="28">
+      <c r="H10" s="32">
+        <f>'[1]20240410_趙入力'!$AE$16/11</f>
+        <v>28.428805194805193</v>
+      </c>
+      <c r="I10" s="29">
         <f>H10*10</f>
-        <v>113.75851146787994</v>
-      </c>
-      <c r="J10" s="28">
-        <f>K10*$H$55</f>
-        <v>4.5351689999999995E-3</v>
-      </c>
-      <c r="K10" s="28">
-        <f>K4+K7</f>
-        <v>0.15117229999999998</v>
+        <v>284.28805194805193</v>
+      </c>
+      <c r="J10" s="32">
+        <f>'[1]20240410_趙入力'!$AC$16</f>
+        <v>2.6998400000000002E-4</v>
+      </c>
+      <c r="K10" s="29">
+        <f>'[1]20240410_趙入力'!$AA$5</f>
+        <v>0.12272000000000001</v>
       </c>
       <c r="L10" s="28">
         <v>0</v>
       </c>
-      <c r="M10" s="28">
-        <f>$E$59*N10</f>
-        <v>2755.9670190672905</v>
-      </c>
-      <c r="N10" s="29">
-        <f>[1]趙メモ!$P$16</f>
-        <v>3.2170000000000002E-3</v>
+      <c r="M10" s="32">
+        <f>'[1]20240410_趙入力'!$AB$16</f>
+        <v>1009.8833333333332</v>
+      </c>
+      <c r="N10" s="32">
+        <f>'[1]20240410_趙入力'!$H$36</f>
+        <v>3.1438E-3</v>
       </c>
       <c r="O10" s="28">
         <v>8</v>
@@ -2393,32 +3513,31 @@
       <c r="G11">
         <v>0</v>
       </c>
-      <c r="H11">
-        <f>$H$47*N11/11</f>
-        <v>2.1653624259306707</v>
-      </c>
-      <c r="I11">
+      <c r="H11" s="34">
+        <f>H8/2</f>
+        <v>3.7054642857142857</v>
+      </c>
+      <c r="I11" s="3">
         <f t="shared" ref="I11:I12" si="1">H11*10</f>
-        <v>21.653624259306707</v>
-      </c>
-      <c r="J11">
-        <f>K11*$H$41</f>
-        <v>1.0623543572460281E-3</v>
-      </c>
-      <c r="K11">
-        <f>$C$47*N11</f>
-        <v>0.1062354357246028</v>
+        <v>37.054642857142859</v>
+      </c>
+      <c r="J11" s="34">
+        <f>J8/2</f>
+        <v>1.44716E-4</v>
+      </c>
+      <c r="K11" s="34">
+        <f>K8/2</f>
+        <v>6.5780000000000005E-2</v>
       </c>
       <c r="L11">
         <v>0</v>
       </c>
-      <c r="M11">
-        <f>$E$45*N11</f>
-        <v>530.26209484833942</v>
-      </c>
-      <c r="N11" s="3">
-        <f>[1]趙メモ!$F$33</f>
-        <v>2.3800705916400002E-3</v>
+      <c r="M11" s="34">
+        <f>$M$5/2</f>
+        <v>498.14645833333316</v>
+      </c>
+      <c r="N11">
+        <v>4.0000000000000002E-4</v>
       </c>
       <c r="O11">
         <v>0.15</v>
@@ -2442,7 +3561,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A12">
         <v>1</v>
       </c>
@@ -2464,30 +3583,30 @@
       <c r="G12">
         <v>0</v>
       </c>
-      <c r="H12">
-        <f>$H$47*N12/11</f>
-        <v>0</v>
-      </c>
-      <c r="I12">
+      <c r="H12" s="34">
+        <f>H8/2</f>
+        <v>3.7054642857142857</v>
+      </c>
+      <c r="I12" s="3">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J12">
-        <f t="shared" ref="J12" si="2">K12*$H$41</f>
-        <v>0</v>
-      </c>
-      <c r="K12">
-        <f t="shared" ref="K12" si="3">$C$47*N12</f>
-        <v>0</v>
+        <v>37.054642857142859</v>
+      </c>
+      <c r="J12" s="34">
+        <f>J8/2</f>
+        <v>1.44716E-4</v>
+      </c>
+      <c r="K12" s="34">
+        <f>K8/2</f>
+        <v>6.5780000000000005E-2</v>
       </c>
       <c r="L12">
         <v>0</v>
       </c>
-      <c r="M12">
-        <f t="shared" ref="M12" si="4">$E$45*N12</f>
-        <v>0</v>
-      </c>
-      <c r="N12" s="3">
+      <c r="M12" s="34">
+        <f>$M$5/2</f>
+        <v>498.14645833333316</v>
+      </c>
+      <c r="N12">
         <v>0</v>
       </c>
       <c r="O12">
@@ -2534,32 +3653,31 @@
       <c r="G13">
         <v>0</v>
       </c>
-      <c r="H13">
-        <f>N13*$H$75/11</f>
-        <v>0.52508830944758855</v>
-      </c>
-      <c r="I13">
+      <c r="H13" s="34">
+        <f>'[1]20240410_趙入力'!$AE$23/11</f>
+        <v>6.9075779220779223</v>
+      </c>
+      <c r="I13" s="3">
         <f>H13*10</f>
-        <v>5.2508830944758857</v>
-      </c>
-      <c r="J13">
-        <f>K13*$H$69</f>
-        <v>1.2129539948239304E-3</v>
-      </c>
-      <c r="K13">
-        <f>$C$75*N13</f>
-        <v>0.14555447937887164</v>
+        <v>69.075779220779225</v>
+      </c>
+      <c r="J13" s="34">
+        <f>'[1]20240410_趙入力'!$AC$23</f>
+        <v>2.2448800000000001E-4</v>
+      </c>
+      <c r="K13" s="3">
+        <f>'[1]20240410_趙入力'!$AA$11</f>
+        <v>0.10204000000000001</v>
       </c>
       <c r="L13">
         <v>0</v>
       </c>
-      <c r="M13">
-        <f>$E$73*N13</f>
-        <v>1063.805577682617</v>
-      </c>
-      <c r="N13" s="3">
-        <f>[1]趙メモ!$K$33</f>
-        <v>3.1450484019150001E-3</v>
+      <c r="M13" s="34">
+        <f>'[1]20240410_趙入力'!$AB$23</f>
+        <v>737.66416666666555</v>
+      </c>
+      <c r="N13">
+        <v>5.0000000000000001E-4</v>
       </c>
       <c r="O13">
         <v>0.2</v>
@@ -2605,32 +3723,32 @@
       <c r="G14" s="28">
         <v>0</v>
       </c>
-      <c r="H14" s="28">
-        <f>($H$61*N14)/11</f>
-        <v>10.315000868878016</v>
-      </c>
-      <c r="I14" s="28">
+      <c r="H14" s="32">
+        <f>'[1]20240410_趙入力'!$AE$15/11</f>
+        <v>25.839272727272725</v>
+      </c>
+      <c r="I14" s="29">
         <f>H14*10</f>
-        <v>103.15000868878016</v>
-      </c>
-      <c r="J14" s="28">
-        <f>K14*$H$55</f>
-        <v>6.6703379999999987E-3</v>
-      </c>
-      <c r="K14" s="28">
-        <f>K10+K7</f>
-        <v>0.22234459999999998</v>
+        <v>258.39272727272726</v>
+      </c>
+      <c r="J14" s="32">
+        <f>'[1]20240410_趙入力'!$AC$15</f>
+        <v>1.9219200000000002E-4</v>
+      </c>
+      <c r="K14" s="29">
+        <f>'[1]20240410_趙入力'!$AA$4</f>
+        <v>8.7360000000000007E-2</v>
       </c>
       <c r="L14" s="28">
         <v>0</v>
       </c>
-      <c r="M14" s="28">
-        <f>$E$59*N14</f>
-        <v>2498.9604583833657</v>
-      </c>
-      <c r="N14" s="29">
-        <f>[1]趙メモ!$P$15</f>
-        <v>2.9170000000000003E-3</v>
+      <c r="M14" s="32">
+        <f>'[1]20240410_趙入力'!$AB$15</f>
+        <v>777.13999999999942</v>
+      </c>
+      <c r="N14" s="32">
+        <f>'[1]20240410_趙入力'!$H$35</f>
+        <v>2.6849999999999999E-3</v>
       </c>
       <c r="O14" s="28">
         <v>15</v>
@@ -2676,32 +3794,31 @@
       <c r="G15">
         <v>0</v>
       </c>
-      <c r="H15">
-        <f>$H$47*N15/11</f>
-        <v>1.7471525128338179</v>
-      </c>
-      <c r="I15">
-        <f t="shared" ref="I15:I16" si="5">H15*10</f>
-        <v>17.471525128338179</v>
-      </c>
-      <c r="J15">
-        <f t="shared" ref="J15:J16" si="6">K15*$H$41</f>
-        <v>8.5717525276841607E-4</v>
-      </c>
-      <c r="K15">
-        <f t="shared" ref="K15:K16" si="7">$C$47*N15</f>
-        <v>8.5717525276841608E-2</v>
+      <c r="H15" s="34">
+        <f>H8/2</f>
+        <v>3.7054642857142857</v>
+      </c>
+      <c r="I15" s="3">
+        <f t="shared" ref="I15:I16" si="2">H15*10</f>
+        <v>37.054642857142859</v>
+      </c>
+      <c r="J15" s="34">
+        <f>J8/2</f>
+        <v>1.44716E-4</v>
+      </c>
+      <c r="K15" s="34">
+        <f>K8/2</f>
+        <v>6.5780000000000005E-2</v>
       </c>
       <c r="L15">
         <v>0</v>
       </c>
-      <c r="M15">
-        <f t="shared" ref="M15:M16" si="8">$E$45*N15</f>
-        <v>427.84927843042885</v>
-      </c>
-      <c r="N15" s="3">
-        <f>[1]趙メモ!$F$32*0.8</f>
-        <v>1.9203927550920001E-3</v>
+      <c r="M15" s="34">
+        <f>$M$5/2</f>
+        <v>498.14645833333316</v>
+      </c>
+      <c r="N15">
+        <v>4.0000000000000002E-4</v>
       </c>
       <c r="O15">
         <v>0.5</v>
@@ -2747,32 +3864,31 @@
       <c r="G16">
         <v>0</v>
       </c>
-      <c r="H16">
-        <f>$H$47*N16/11</f>
-        <v>0.43678812820845447</v>
-      </c>
-      <c r="I16">
-        <f t="shared" si="5"/>
-        <v>4.3678812820845447</v>
-      </c>
-      <c r="J16">
-        <f t="shared" si="6"/>
-        <v>2.1429381319210402E-4</v>
-      </c>
-      <c r="K16">
-        <f t="shared" si="7"/>
-        <v>2.1429381319210402E-2</v>
+      <c r="H16" s="34">
+        <f>H8/2</f>
+        <v>3.7054642857142857</v>
+      </c>
+      <c r="I16" s="3">
+        <f t="shared" si="2"/>
+        <v>37.054642857142859</v>
+      </c>
+      <c r="J16" s="34">
+        <f>J8/2</f>
+        <v>1.44716E-4</v>
+      </c>
+      <c r="K16" s="34">
+        <f>K8/2</f>
+        <v>6.5780000000000005E-2</v>
       </c>
       <c r="L16">
         <v>0</v>
       </c>
-      <c r="M16">
-        <f t="shared" si="8"/>
-        <v>106.96231960760721</v>
-      </c>
-      <c r="N16" s="3">
-        <f>[1]趙メモ!$F$32*0.2</f>
-        <v>4.8009818877300004E-4</v>
+      <c r="M16" s="34">
+        <f>$M$5/2</f>
+        <v>498.14645833333316</v>
+      </c>
+      <c r="N16">
+        <v>8.0000000000000007E-5</v>
       </c>
       <c r="O16">
         <v>0.5</v>
@@ -2796,7 +3912,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:25" x14ac:dyDescent="0.4">
       <c r="A17">
         <v>1</v>
       </c>
@@ -2818,32 +3934,31 @@
       <c r="G17">
         <v>0</v>
       </c>
-      <c r="H17">
-        <f>N17*$H$75/11</f>
-        <v>0.47940337112685644</v>
-      </c>
-      <c r="I17">
+      <c r="H17" s="34">
+        <f>'[1]20240410_趙入力'!$AE$23/11</f>
+        <v>6.9075779220779223</v>
+      </c>
+      <c r="I17" s="3">
         <f>H17*10</f>
-        <v>4.7940337112685647</v>
-      </c>
-      <c r="J17">
-        <f>K17*$H$69</f>
-        <v>1.1074217873030393E-3</v>
-      </c>
-      <c r="K17">
-        <f>$C$75*N17</f>
-        <v>0.13289061447636472</v>
+        <v>69.075779220779225</v>
+      </c>
+      <c r="J17" s="34">
+        <f>'[1]20240410_趙入力'!$AC$23</f>
+        <v>2.2448800000000001E-4</v>
+      </c>
+      <c r="K17" s="3">
+        <f>'[1]20240410_趙入力'!$AA$11</f>
+        <v>0.10204000000000001</v>
       </c>
       <c r="L17">
         <v>0</v>
       </c>
-      <c r="M17">
-        <f>$E$73*N17</f>
-        <v>971.2499230865169</v>
-      </c>
-      <c r="N17" s="3">
-        <f>[1]趙メモ!$K$32</f>
-        <v>2.8714156821000006E-3</v>
+      <c r="M17" s="34">
+        <f>$M$6</f>
+        <v>737.66416666666555</v>
+      </c>
+      <c r="N17">
+        <v>5.9999999999999995E-4</v>
       </c>
       <c r="O17">
         <v>0.5</v>
@@ -2867,7 +3982,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:25" x14ac:dyDescent="0.4">
       <c r="A18">
         <v>1</v>
       </c>
@@ -2904,7 +4019,7 @@
       <c r="L18">
         <v>0</v>
       </c>
-      <c r="M18">
+      <c r="M18" s="33">
         <v>0</v>
       </c>
       <c r="N18">
@@ -2932,7 +4047,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:25" x14ac:dyDescent="0.4">
       <c r="A19">
         <v>1</v>
       </c>
@@ -2997,7 +4112,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:25" x14ac:dyDescent="0.4">
       <c r="A20">
         <v>1</v>
       </c>
@@ -3019,23 +4134,28 @@
       <c r="G20">
         <v>0</v>
       </c>
-      <c r="H20">
-        <v>24</v>
-      </c>
-      <c r="I20">
-        <v>243</v>
-      </c>
-      <c r="J20">
-        <v>1.013E-3</v>
-      </c>
-      <c r="K20">
-        <v>0.21</v>
+      <c r="H20" s="34">
+        <f>'[1]20240410_趙入力'!$AE$21/11</f>
+        <v>25.208000000000002</v>
+      </c>
+      <c r="I20" s="34">
+        <f>H20*10</f>
+        <v>252.08</v>
+      </c>
+      <c r="J20" s="34">
+        <f>'[1]20240410_趙入力'!$AC$21</f>
+        <v>3.3756800000000006E-4</v>
+      </c>
+      <c r="K20" s="34">
+        <f>'[1]20240410_趙入力'!$AA$10</f>
+        <v>0.15344000000000002</v>
       </c>
       <c r="L20">
         <v>0</v>
       </c>
-      <c r="M20">
-        <v>726</v>
+      <c r="M20" s="34">
+        <f>'[1]20240410_趙入力'!$AB$21</f>
+        <v>1.5983333333324481</v>
       </c>
       <c r="N20" s="24">
         <v>1.5E-3</v>
@@ -3062,63 +4182,39 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:21" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A22" s="18" t="s">
-        <v>54</v>
-      </c>
+    <row r="22" spans="1:25" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A22" s="18"/>
       <c r="C22" s="11"/>
       <c r="D22" s="11"/>
       <c r="E22" s="11"/>
       <c r="F22" s="11"/>
     </row>
-    <row r="23" spans="1:21" x14ac:dyDescent="0.4">
-      <c r="A23" s="19" t="s">
-        <v>32</v>
-      </c>
+    <row r="23" spans="1:25" x14ac:dyDescent="0.4">
+      <c r="A23" s="19"/>
       <c r="B23" s="6"/>
       <c r="C23" s="5"/>
       <c r="G23" s="6"/>
-      <c r="H23" s="15" t="s">
-        <v>41</v>
-      </c>
+      <c r="H23" s="15"/>
       <c r="I23" s="6"/>
       <c r="J23" s="6"/>
       <c r="K23" s="6"/>
       <c r="L23" s="7"/>
     </row>
-    <row r="24" spans="1:21" x14ac:dyDescent="0.4">
-      <c r="A24" s="20">
-        <f>[2]CNデータ!$G$11*1000</f>
-        <v>15212.166666666664</v>
-      </c>
+    <row r="24" spans="1:25" x14ac:dyDescent="0.4">
+      <c r="A24" s="31"/>
       <c r="B24" s="5"/>
-      <c r="C24" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="E24" t="s">
-        <v>65</v>
-      </c>
+      <c r="C24" s="5"/>
       <c r="G24" s="5"/>
-      <c r="H24" s="14">
-        <f>[2]CNデータ!$J$11*1000</f>
-        <v>350.44285714285718</v>
-      </c>
+      <c r="H24" s="30"/>
       <c r="I24" s="5"/>
       <c r="J24" s="5"/>
       <c r="K24" s="5"/>
       <c r="L24" s="9"/>
     </row>
-    <row r="25" spans="1:21" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:25" x14ac:dyDescent="0.4">
       <c r="A25" s="8"/>
       <c r="B25" s="5"/>
-      <c r="C25" s="5">
-        <f>H20*14/0.135*0.38/12+I20*14/0.151*0.38/12+M20+K20*0.44/12*1000000</f>
-        <v>9218.2585234240851</v>
-      </c>
-      <c r="E25">
-        <f>A24-C25</f>
-        <v>5993.9081432425792</v>
-      </c>
+      <c r="C25" s="5"/>
       <c r="F25" s="5"/>
       <c r="G25" s="5"/>
       <c r="H25" s="5"/>
@@ -3127,60 +4223,43 @@
       <c r="K25" s="5"/>
       <c r="L25" s="9"/>
     </row>
-    <row r="26" spans="1:21" x14ac:dyDescent="0.4">
-      <c r="A26" s="21" t="s">
-        <v>55</v>
-      </c>
+    <row r="26" spans="1:25" x14ac:dyDescent="0.4">
+      <c r="A26" s="21"/>
       <c r="B26" s="5"/>
       <c r="C26" s="5"/>
       <c r="D26" s="5"/>
       <c r="F26" s="5"/>
       <c r="G26" s="5"/>
-      <c r="H26" s="5" t="s">
-        <v>68</v>
-      </c>
+      <c r="H26" s="5"/>
       <c r="I26" s="5"/>
       <c r="J26" s="5"/>
       <c r="K26" s="5"/>
       <c r="L26" s="9"/>
       <c r="N26" s="3" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="27" spans="1:21" x14ac:dyDescent="0.4">
-      <c r="A27" s="22">
-        <f>[2]CNデータ!$C$11/5</f>
-        <v>0.442</v>
-      </c>
+        <v>63</v>
+      </c>
+    </row>
+    <row r="27" spans="1:25" x14ac:dyDescent="0.4">
+      <c r="A27" s="22"/>
       <c r="B27" s="5"/>
       <c r="C27" s="5"/>
       <c r="D27" s="5"/>
-      <c r="E27" t="s">
-        <v>67</v>
-      </c>
       <c r="G27" s="5"/>
-      <c r="H27" s="5">
-        <f>J20/14*1000000</f>
-        <v>72.357142857142861</v>
-      </c>
+      <c r="H27" s="5"/>
       <c r="I27" s="5"/>
       <c r="J27" s="5"/>
       <c r="K27" s="5"/>
       <c r="L27" s="9"/>
       <c r="N27" s="4">
-        <f>SUM(A27,A42,A56,A70)*0.8</f>
-        <v>2.4214400000000005</v>
-      </c>
-    </row>
-    <row r="28" spans="1:21" x14ac:dyDescent="0.4">
+        <f>SUM(A27,A42,X69,A56)*0.8</f>
+        <v>2.0348800000000002</v>
+      </c>
+    </row>
+    <row r="28" spans="1:25" x14ac:dyDescent="0.4">
       <c r="A28" s="8"/>
       <c r="B28" s="5"/>
       <c r="C28" s="5"/>
       <c r="D28" s="5"/>
-      <c r="E28">
-        <f>A27-K20</f>
-        <v>0.23200000000000001</v>
-      </c>
       <c r="G28" s="5"/>
       <c r="H28" s="5"/>
       <c r="I28" s="5"/>
@@ -3188,31 +4267,67 @@
       <c r="K28" s="5"/>
       <c r="L28" s="9"/>
     </row>
-    <row r="29" spans="1:21" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:25" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A29" s="20"/>
       <c r="B29" s="5"/>
       <c r="D29" s="5"/>
       <c r="E29" s="5"/>
       <c r="F29" s="5"/>
       <c r="G29" s="5"/>
-      <c r="H29" s="5" t="s">
-        <v>69</v>
-      </c>
+      <c r="H29" s="5"/>
       <c r="I29" s="5"/>
       <c r="J29" s="5"/>
       <c r="K29" s="5"/>
       <c r="L29" s="9"/>
-    </row>
-    <row r="30" spans="1:21" x14ac:dyDescent="0.4">
+      <c r="R29" t="s">
+        <v>67</v>
+      </c>
+      <c r="S29">
+        <v>0</v>
+      </c>
+      <c r="T29">
+        <v>120</v>
+      </c>
+      <c r="U29">
+        <v>288</v>
+      </c>
+      <c r="V29">
+        <v>480</v>
+      </c>
+      <c r="W29">
+        <v>648</v>
+      </c>
+      <c r="X29">
+        <v>816</v>
+      </c>
+    </row>
+    <row r="30" spans="1:25" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A30" s="13"/>
       <c r="B30" s="5"/>
-      <c r="H30">
-        <f>H24-H20-I20</f>
-        <v>83.442857142857179</v>
-      </c>
       <c r="L30" s="9"/>
-    </row>
-    <row r="31" spans="1:21" x14ac:dyDescent="0.4">
+      <c r="S30" s="35">
+        <v>2.6849999999999999E-3</v>
+      </c>
+      <c r="T30" s="35">
+        <v>2.9581999999999981E-3</v>
+      </c>
+      <c r="U30" s="35">
+        <v>2.9004E-3</v>
+      </c>
+      <c r="V30" s="35">
+        <v>1.3575999999999998E-3</v>
+      </c>
+      <c r="W30" s="35">
+        <v>3.4460000000000003E-4</v>
+      </c>
+      <c r="X30" s="35">
+        <v>4.77999999999998E-5</v>
+      </c>
+      <c r="Y30">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="31" spans="1:25" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A31" s="8"/>
       <c r="B31" s="5"/>
       <c r="C31" s="5"/>
@@ -3225,11 +4340,30 @@
       <c r="J31" s="5"/>
       <c r="K31" s="5"/>
       <c r="L31" s="9"/>
-    </row>
-    <row r="32" spans="1:21" x14ac:dyDescent="0.4">
-      <c r="A32" s="26" t="s">
-        <v>45</v>
-      </c>
+      <c r="S31">
+        <v>3.1438E-3</v>
+      </c>
+      <c r="T31" s="35">
+        <v>2.9265999999999997E-3</v>
+      </c>
+      <c r="U31" s="35">
+        <v>1.9917999999999997E-3</v>
+      </c>
+      <c r="V31">
+        <v>0</v>
+      </c>
+      <c r="W31">
+        <v>0</v>
+      </c>
+      <c r="X31">
+        <v>0</v>
+      </c>
+      <c r="Y31">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="32" spans="1:25" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A32" s="26"/>
       <c r="B32" s="5"/>
       <c r="C32" s="5"/>
       <c r="D32" s="5"/>
@@ -3241,12 +4375,30 @@
       <c r="J32" s="5"/>
       <c r="K32" s="5"/>
       <c r="L32" s="9"/>
-    </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.4">
-      <c r="A33" s="27">
-        <f>SUM(N20)</f>
-        <v>1.5E-3</v>
-      </c>
+      <c r="S32">
+        <v>2.7525999999999996E-3</v>
+      </c>
+      <c r="T32" s="35">
+        <v>2.0139999999999997E-3</v>
+      </c>
+      <c r="U32">
+        <v>0</v>
+      </c>
+      <c r="V32">
+        <v>0</v>
+      </c>
+      <c r="W32">
+        <v>0</v>
+      </c>
+      <c r="X32">
+        <v>0</v>
+      </c>
+      <c r="Y32">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="33" spans="1:25" x14ac:dyDescent="0.4">
+      <c r="A33" s="27"/>
       <c r="B33" s="5"/>
       <c r="C33" s="14"/>
       <c r="D33" s="5"/>
@@ -3258,8 +4410,29 @@
       <c r="J33" s="5"/>
       <c r="K33" s="5"/>
       <c r="L33" s="9"/>
-    </row>
-    <row r="34" spans="1:17" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="S33">
+        <v>1.4895999999999998E-3</v>
+      </c>
+      <c r="T33" s="35">
+        <v>1.5459999999999998E-3</v>
+      </c>
+      <c r="U33">
+        <v>0</v>
+      </c>
+      <c r="V33">
+        <v>0</v>
+      </c>
+      <c r="W33">
+        <v>0</v>
+      </c>
+      <c r="X33">
+        <v>0</v>
+      </c>
+      <c r="Y33">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="34" spans="1:25" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A34" s="10"/>
       <c r="B34" s="11"/>
       <c r="C34" s="11"/>
@@ -3273,10 +4446,20 @@
       <c r="K34" s="11"/>
       <c r="L34" s="12"/>
     </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:25" x14ac:dyDescent="0.4">
       <c r="A35" s="3"/>
     </row>
-    <row r="37" spans="1:17" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:25" x14ac:dyDescent="0.4">
+      <c r="V36" s="36">
+        <f>0.531/3</f>
+        <v>0.17700000000000002</v>
+      </c>
+      <c r="W36" s="36">
+        <f>1.354/3</f>
+        <v>0.45133333333333336</v>
+      </c>
+    </row>
+    <row r="37" spans="1:25" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A37" s="18" t="s">
         <v>53</v>
       </c>
@@ -3285,13 +4468,13 @@
       <c r="E37" s="11"/>
       <c r="F37" s="11"/>
     </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:25" x14ac:dyDescent="0.4">
       <c r="A38" s="19" t="s">
         <v>32</v>
       </c>
       <c r="B38" s="6"/>
       <c r="C38" s="5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="G38" s="6"/>
       <c r="H38" s="15" t="s">
@@ -3302,41 +4485,40 @@
       <c r="K38" s="6"/>
       <c r="L38" s="7"/>
       <c r="N38" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="P38" t="s">
         <v>56</v>
       </c>
-      <c r="P38" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.4">
-      <c r="A39" s="20">
-        <f>[2]CNデータ!$G$10*1000</f>
-        <v>22723.325000000004</v>
+    </row>
+    <row r="39" spans="1:25" x14ac:dyDescent="0.4">
+      <c r="A39" s="31">
+        <f>'[1]20240410_趙入力'!$X$20</f>
+        <v>23280.638333333332</v>
       </c>
       <c r="B39" s="5"/>
       <c r="C39" s="5">
         <f>A39-P39</f>
-        <v>14559.489500000003</v>
+        <v>22449.638333333332</v>
       </c>
       <c r="G39" s="5"/>
-      <c r="H39" s="14">
-        <f>[2]CNデータ!$J$10*1000</f>
-        <v>374.46428571428567</v>
+      <c r="H39" s="30">
+        <f>'[1]20240410_趙入力'!$Y$20</f>
+        <v>408.77571428571429</v>
       </c>
       <c r="I39" s="5"/>
       <c r="J39" s="5"/>
       <c r="K39" s="5"/>
       <c r="L39" s="9"/>
       <c r="N39" s="4">
-        <f>SUM(A39,A53,A67)</f>
-        <v>81638.35500000001</v>
+        <f>SUM(A39,X66,A53)</f>
+        <v>69354.32166666667</v>
       </c>
       <c r="P39">
-        <f>N39/10</f>
-        <v>8163.835500000001</v>
-      </c>
-    </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.4">
+        <v>831</v>
+      </c>
+    </row>
+    <row r="40" spans="1:25" x14ac:dyDescent="0.4">
       <c r="A40" s="8"/>
       <c r="B40" s="5"/>
       <c r="C40" s="5"/>
@@ -3352,7 +4534,7 @@
       <c r="K40" s="5"/>
       <c r="L40" s="9"/>
     </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:25" x14ac:dyDescent="0.4">
       <c r="A41" s="21" t="s">
         <v>30</v>
       </c>
@@ -3361,7 +4543,7 @@
       <c r="D41" s="5"/>
       <c r="F41" s="5">
         <f>C45*0.44/12*1000000</f>
-        <v>12815.000000000002</v>
+        <v>10853.7</v>
       </c>
       <c r="G41" s="5"/>
       <c r="H41" s="5">
@@ -3373,13 +4555,13 @@
       <c r="K41" s="5"/>
       <c r="L41" s="9"/>
       <c r="N41" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.4">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="42" spans="1:25" x14ac:dyDescent="0.4">
       <c r="A42" s="22">
-        <f>[2]CNデータ!$C$10/5</f>
-        <v>0.69900000000000007</v>
+        <f>'[1]20240410_趙入力'!$Z$9</f>
+        <v>0.65780000000000005</v>
       </c>
       <c r="B42" s="5"/>
       <c r="C42" s="5" t="s">
@@ -3404,7 +4586,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="43" spans="1:25" x14ac:dyDescent="0.4">
       <c r="A43" s="8"/>
       <c r="B43" s="5"/>
       <c r="C43" s="5">
@@ -3413,23 +4595,23 @@
       <c r="D43" s="5"/>
       <c r="E43">
         <f>A45-C45</f>
-        <v>0.42716666666666669</v>
+        <v>0.43487888888888887</v>
       </c>
       <c r="F43">
         <f>C39-F41</f>
-        <v>1744.4895000000015</v>
+        <v>11595.938333333332</v>
       </c>
       <c r="G43" s="5"/>
       <c r="H43" s="5">
         <f>SUM(J5,J8,J11,J12,J15,J16)/14*1000000</f>
-        <v>249.6428571428572</v>
+        <v>82.694857142857146</v>
       </c>
       <c r="I43" s="5"/>
       <c r="J43" s="5"/>
       <c r="K43" s="5"/>
       <c r="L43" s="9"/>
     </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="44" spans="1:25" x14ac:dyDescent="0.4">
       <c r="A44" s="20" t="s">
         <v>38</v>
       </c>
@@ -3448,43 +4630,43 @@
       </c>
       <c r="I44" s="5"/>
       <c r="J44" s="5" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="K44" s="5"/>
       <c r="L44" s="9"/>
       <c r="N44" s="24" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.4">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="45" spans="1:25" x14ac:dyDescent="0.4">
       <c r="A45" s="13">
         <f>A42*5/4.5</f>
-        <v>0.77666666666666673</v>
+        <v>0.73088888888888892</v>
       </c>
       <c r="B45" s="5"/>
       <c r="C45">
-        <f>A45*C43</f>
-        <v>0.34950000000000003</v>
+        <f>A42*C43</f>
+        <v>0.29601000000000005</v>
       </c>
       <c r="E45">
         <f>F43/A48</f>
-        <v>222792.59140921509</v>
+        <v>9427592.1409214083</v>
       </c>
       <c r="H45">
         <f>H39-H43</f>
-        <v>124.82142857142847</v>
+        <v>326.08085714285716</v>
       </c>
       <c r="J45">
         <f>H45-Q48</f>
-        <v>78.361196428571333</v>
+        <v>151.09700000000001</v>
       </c>
       <c r="L45" s="9"/>
       <c r="N45" s="25">
-        <f>SUM(H45,H59,H73)</f>
-        <v>557.52278571428565</v>
-      </c>
-    </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.4">
+        <f>SUM(H45,AE72,H59)</f>
+        <v>2099.8062857142859</v>
+      </c>
+    </row>
+    <row r="46" spans="1:25" x14ac:dyDescent="0.4">
       <c r="A46" s="8"/>
       <c r="B46" s="5"/>
       <c r="C46" s="5" t="s">
@@ -3502,14 +4684,14 @@
       <c r="K46" s="5"/>
       <c r="L46" s="9"/>
     </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="47" spans="1:25" x14ac:dyDescent="0.4">
       <c r="A47" s="20" t="s">
         <v>45</v>
       </c>
       <c r="B47" s="5"/>
       <c r="C47" s="5">
         <f>C45/A48</f>
-        <v>44.635413797286034</v>
+        <v>240.65853658536591</v>
       </c>
       <c r="D47" s="5"/>
       <c r="E47" s="5"/>
@@ -3517,23 +4699,23 @@
       <c r="G47" s="5"/>
       <c r="H47" s="5">
         <f>J45/A48</f>
-        <v>10007.680767495547</v>
+        <v>122843.08943089432</v>
       </c>
       <c r="I47" s="5"/>
       <c r="J47" s="5"/>
       <c r="K47" s="5"/>
       <c r="L47" s="9"/>
       <c r="N47" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="Q47" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.4">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="48" spans="1:25" x14ac:dyDescent="0.4">
       <c r="A48" s="20">
         <f>SUM(N5,N8,N11,N15,N16,N12)</f>
-        <v>7.8301055208600014E-3</v>
+        <v>1.23E-3</v>
       </c>
       <c r="B48" s="5"/>
       <c r="C48" s="14"/>
@@ -3551,10 +4733,10 @@
       </c>
       <c r="Q48">
         <f>N45/(N48+N48+N51)</f>
-        <v>46.460232142857137</v>
-      </c>
-    </row>
-    <row r="49" spans="1:15" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
+        <v>174.98385714285715</v>
+      </c>
+    </row>
+    <row r="49" spans="1:29" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A49" s="10"/>
       <c r="B49" s="11"/>
       <c r="C49" s="11"/>
@@ -3568,14 +4750,14 @@
       <c r="K49" s="11"/>
       <c r="L49" s="12"/>
     </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="50" spans="1:29" x14ac:dyDescent="0.4">
       <c r="N50" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="51" spans="1:15" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="51" spans="1:29" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A51" s="17" t="s">
-        <v>31</v>
+        <v>49</v>
       </c>
       <c r="C51" s="11"/>
       <c r="D51" s="11"/>
@@ -3585,14 +4767,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="52" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="52" spans="1:29" x14ac:dyDescent="0.4">
       <c r="A52" s="13" t="s">
         <v>32</v>
       </c>
       <c r="B52" s="6"/>
-      <c r="C52" s="5" t="s">
-        <v>46</v>
-      </c>
+      <c r="C52" s="5"/>
       <c r="G52" s="6"/>
       <c r="H52" s="15" t="s">
         <v>41</v>
@@ -3602,30 +4782,26 @@
       <c r="K52" s="6"/>
       <c r="L52" s="7"/>
     </row>
-    <row r="53" spans="1:15" x14ac:dyDescent="0.4">
-      <c r="A53" s="14">
-        <f>[2]CNデータ!$G$8*1000</f>
-        <v>28157.160000000007</v>
-      </c>
-      <c r="C53" s="5">
-        <v>0.08</v>
-      </c>
+    <row r="53" spans="1:29" x14ac:dyDescent="0.4">
+      <c r="A53" s="30">
+        <f>'[1]20240410_趙入力'!$X$19</f>
+        <v>17916.523333333331</v>
+      </c>
+      <c r="C53" s="5"/>
       <c r="G53" s="5"/>
-      <c r="H53" s="14">
-        <f>[2]CNデータ!$J$8*1000</f>
-        <v>1529.28</v>
+      <c r="H53" s="30">
+        <f>'[1]20240410_趙入力'!$Y$19</f>
+        <v>368.07285714285717</v>
       </c>
       <c r="I53" s="5"/>
       <c r="J53" s="5"/>
       <c r="K53" s="5"/>
       <c r="L53" s="9"/>
     </row>
-    <row r="54" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="54" spans="1:29" x14ac:dyDescent="0.4">
       <c r="A54" s="8"/>
       <c r="B54" s="5"/>
-      <c r="C54" s="5" t="s">
-        <v>47</v>
-      </c>
+      <c r="C54" s="5"/>
       <c r="F54" s="5" t="s">
         <v>33</v>
       </c>
@@ -3638,27 +4814,24 @@
       <c r="K54" s="5"/>
       <c r="L54" s="9"/>
       <c r="N54" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="55" spans="1:15" x14ac:dyDescent="0.4">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="55" spans="1:29" x14ac:dyDescent="0.4">
       <c r="A55" s="1" t="s">
         <v>30</v>
       </c>
       <c r="B55" s="5"/>
-      <c r="C55" s="5">
-        <f>(C59-3*C53)/4</f>
-        <v>7.1172299999999994E-2</v>
-      </c>
+      <c r="C55" s="5"/>
       <c r="D55" s="5"/>
       <c r="F55" s="5">
         <f>C59*0.44/12*1000000</f>
-        <v>19238.603999999999</v>
+        <v>27355.680000000004</v>
       </c>
       <c r="G55" s="5"/>
       <c r="H55" s="5">
-        <f>3/100</f>
-        <v>0.03</v>
+        <f>1/120</f>
+        <v>8.3333333333333332E-3</v>
       </c>
       <c r="I55" s="5"/>
       <c r="J55" s="5"/>
@@ -3668,13 +4841,13 @@
         <v>0.03</v>
       </c>
       <c r="O55" s="3" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="56" spans="1:15" x14ac:dyDescent="0.4">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="56" spans="1:29" x14ac:dyDescent="0.4">
       <c r="A56" s="2">
-        <f>[2]CNデータ!$C$8/5</f>
-        <v>0.84960000000000002</v>
+        <f>[2]CNデータ!$C$9/5</f>
+        <v>1.0362</v>
       </c>
       <c r="B56" s="5"/>
       <c r="C56" s="5" t="s">
@@ -3696,7 +4869,7 @@
       <c r="K56" s="5"/>
       <c r="L56" s="9"/>
     </row>
-    <row r="57" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="57" spans="1:29" x14ac:dyDescent="0.4">
       <c r="B57" s="5"/>
       <c r="C57" s="5">
         <v>0.8</v>
@@ -3704,28 +4877,28 @@
       <c r="D57" s="5"/>
       <c r="E57">
         <f>A59-C59</f>
-        <v>0.13117230000000002</v>
+        <v>0.18651600000000002</v>
       </c>
       <c r="F57">
         <f>A53-F55</f>
-        <v>8918.5560000000078</v>
+        <v>-9439.1566666666731</v>
       </c>
       <c r="G57" s="5"/>
       <c r="H57" s="5">
-        <f>SUM(J4,J7,J10,J14)/14*1000000</f>
-        <v>1124.3339999999998</v>
+        <f>SUM(J6,J9,J13,J17)/14*1000000</f>
+        <v>64.139428571428581</v>
       </c>
       <c r="I57" s="5"/>
       <c r="J57" s="5"/>
       <c r="K57" s="5"/>
       <c r="L57" s="9"/>
       <c r="N57" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="58" spans="1:15" x14ac:dyDescent="0.4">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="58" spans="1:29" x14ac:dyDescent="0.4">
       <c r="A58" s="3" t="s">
-        <v>38</v>
+        <v>51</v>
       </c>
       <c r="B58" s="5"/>
       <c r="C58" t="s">
@@ -3748,29 +4921,31 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="59" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="59" spans="1:29" x14ac:dyDescent="0.4">
       <c r="A59" s="4">
-        <f>A62*C62</f>
-        <v>0.65586149999999999</v>
+        <f>A56/5*4.5</f>
+        <v>0.93258000000000008</v>
       </c>
       <c r="C59">
         <f>A59*C57</f>
-        <v>0.52468919999999997</v>
+        <v>0.74606400000000006</v>
       </c>
       <c r="E59">
         <f>F57/A62</f>
-        <v>856688.53561308375</v>
+        <v>-5552445.0980392192</v>
       </c>
       <c r="H59">
         <f>H53-H57</f>
-        <v>404.94600000000014</v>
+        <v>303.93342857142858</v>
       </c>
       <c r="L59" s="9"/>
     </row>
-    <row r="60" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="60" spans="1:29" x14ac:dyDescent="0.4">
       <c r="A60" s="5"/>
       <c r="B60" s="5"/>
-      <c r="C60" s="5"/>
+      <c r="C60" s="5" t="s">
+        <v>52</v>
+      </c>
       <c r="D60" s="5"/>
       <c r="E60" s="5"/>
       <c r="F60" s="5"/>
@@ -3783,13 +4958,14 @@
       <c r="K60" s="5"/>
       <c r="L60" s="9"/>
     </row>
-    <row r="61" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="61" spans="1:29" x14ac:dyDescent="0.4">
       <c r="A61" s="14" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="B61" s="5"/>
-      <c r="C61" s="3" t="s">
-        <v>37</v>
+      <c r="C61" s="5">
+        <f>C59/A62</f>
+        <v>438.86117647058825</v>
       </c>
       <c r="D61" s="5"/>
       <c r="E61" s="5"/>
@@ -3797,22 +4973,20 @@
       <c r="G61" s="5"/>
       <c r="H61" s="5">
         <f>H59/A62</f>
-        <v>38897.843523365846</v>
+        <v>178784.36974789915</v>
       </c>
       <c r="I61" s="5"/>
       <c r="J61" s="5"/>
       <c r="K61" s="5"/>
       <c r="L61" s="9"/>
     </row>
-    <row r="62" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="62" spans="1:29" x14ac:dyDescent="0.4">
       <c r="A62" s="14">
-        <f>SUM(N4,N7,N10,N14)</f>
-        <v>1.04105E-2</v>
+        <f>SUM(N6,N9,N13,N17)</f>
+        <v>1.7000000000000001E-3</v>
       </c>
       <c r="B62" s="5"/>
-      <c r="C62" s="3">
-        <v>63</v>
-      </c>
+      <c r="C62" s="5"/>
       <c r="D62" s="5"/>
       <c r="E62" s="5"/>
       <c r="F62" s="5"/>
@@ -3823,7 +4997,7 @@
       <c r="K62" s="5"/>
       <c r="L62" s="9"/>
     </row>
-    <row r="63" spans="1:15" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:29" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A63" s="11"/>
       <c r="B63" s="11"/>
       <c r="C63" s="11"/>
@@ -3837,249 +5011,257 @@
       <c r="K63" s="11"/>
       <c r="L63" s="12"/>
     </row>
-    <row r="65" spans="1:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A65" s="17" t="s">
-        <v>49</v>
-      </c>
-      <c r="C65" s="11"/>
-      <c r="D65" s="11"/>
-      <c r="E65" s="11"/>
-      <c r="F65" s="11"/>
-    </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A66" s="13" t="s">
+    <row r="64" spans="1:29" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="X64" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="Z64" s="11"/>
+      <c r="AA64" s="11"/>
+      <c r="AB64" s="11"/>
+      <c r="AC64" s="11"/>
+    </row>
+    <row r="65" spans="24:35" x14ac:dyDescent="0.4">
+      <c r="X65" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="B66" s="6"/>
-      <c r="C66" s="5"/>
-      <c r="G66" s="6"/>
-      <c r="H66" s="15" t="s">
+      <c r="Y65" s="6"/>
+      <c r="Z65" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="AD65" s="6"/>
+      <c r="AE65" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="I66" s="6"/>
-      <c r="J66" s="6"/>
-      <c r="K66" s="6"/>
-      <c r="L66" s="7"/>
-    </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A67" s="14">
-        <f>[2]CNデータ!$G$9*1000</f>
-        <v>30757.87</v>
-      </c>
-      <c r="C67" s="5"/>
-      <c r="G67" s="5"/>
-      <c r="H67" s="14">
-        <f>[2]CNデータ!$J$9*1000</f>
-        <v>444.08571428571429</v>
-      </c>
-      <c r="I67" s="5"/>
-      <c r="J67" s="5"/>
-      <c r="K67" s="5"/>
-      <c r="L67" s="9"/>
-    </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A68" s="8"/>
-      <c r="B68" s="5"/>
-      <c r="C68" s="5"/>
-      <c r="F68" s="5" t="s">
+      <c r="AF65" s="6"/>
+      <c r="AG65" s="6"/>
+      <c r="AH65" s="6"/>
+      <c r="AI65" s="7"/>
+    </row>
+    <row r="66" spans="24:35" x14ac:dyDescent="0.4">
+      <c r="X66" s="14">
+        <f>[2]CNデータ!$G$8*1000</f>
+        <v>28157.160000000007</v>
+      </c>
+      <c r="Z66" s="5">
+        <v>0.08</v>
+      </c>
+      <c r="AD66" s="5"/>
+      <c r="AE66" s="14">
+        <f>[2]CNデータ!$J$8*1000</f>
+        <v>1529.28</v>
+      </c>
+      <c r="AF66" s="5"/>
+      <c r="AG66" s="5"/>
+      <c r="AH66" s="5"/>
+      <c r="AI66" s="9"/>
+    </row>
+    <row r="67" spans="24:35" x14ac:dyDescent="0.4">
+      <c r="X67" s="8"/>
+      <c r="Y67" s="5"/>
+      <c r="Z67" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="AC67" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="G68" s="5"/>
-      <c r="H68" s="5" t="s">
+      <c r="AD67" s="5"/>
+      <c r="AE67" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="I68" s="5"/>
-      <c r="J68" s="5"/>
-      <c r="K68" s="5"/>
-      <c r="L68" s="9"/>
-    </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A69" s="1" t="s">
+      <c r="AF67" s="5"/>
+      <c r="AG67" s="5"/>
+      <c r="AH67" s="5"/>
+      <c r="AI67" s="9"/>
+    </row>
+    <row r="68" spans="24:35" x14ac:dyDescent="0.4">
+      <c r="X68" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B69" s="5"/>
-      <c r="C69" s="5"/>
-      <c r="D69" s="5"/>
-      <c r="F69" s="5">
-        <f>C73*0.44/12*1000000</f>
-        <v>25645.95</v>
-      </c>
-      <c r="G69" s="5"/>
-      <c r="H69" s="5">
-        <f>1/120</f>
-        <v>8.3333333333333332E-3</v>
-      </c>
-      <c r="I69" s="5"/>
-      <c r="J69" s="5"/>
-      <c r="K69" s="5"/>
-      <c r="L69" s="9"/>
-    </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A70" s="2">
-        <f>[2]CNデータ!$C$9/5</f>
-        <v>1.0362</v>
-      </c>
-      <c r="B70" s="5"/>
-      <c r="C70" s="5" t="s">
+      <c r="Y68" s="5"/>
+      <c r="Z68" s="5">
+        <f>(Z72-3*Z66)/4</f>
+        <v>6.6894599999999999E-2</v>
+      </c>
+      <c r="AA68" s="5"/>
+      <c r="AC68" s="5">
+        <f>Z72*0.44/12*1000000</f>
+        <v>18611.208000000002</v>
+      </c>
+      <c r="AD68" s="5"/>
+      <c r="AE68" s="5">
+        <f>3/100</f>
+        <v>0.03</v>
+      </c>
+      <c r="AF68" s="5"/>
+      <c r="AG68" s="5"/>
+      <c r="AH68" s="5"/>
+      <c r="AI68" s="9"/>
+    </row>
+    <row r="69" spans="24:35" x14ac:dyDescent="0.4">
+      <c r="X69" s="2">
+        <f>[2]CNデータ!$C$8/5</f>
+        <v>0.84960000000000002</v>
+      </c>
+      <c r="Y69" s="5"/>
+      <c r="Z69" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="D70" s="5"/>
-      <c r="E70" t="s">
+      <c r="AA69" s="5"/>
+      <c r="AB69" t="s">
         <v>35</v>
       </c>
-      <c r="F70" t="s">
+      <c r="AC69" t="s">
         <v>36</v>
       </c>
-      <c r="G70" s="5"/>
-      <c r="H70" s="16" t="s">
+      <c r="AD69" s="5"/>
+      <c r="AE69" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="I70" s="5"/>
-      <c r="J70" s="5"/>
-      <c r="K70" s="5"/>
-      <c r="L70" s="9"/>
-    </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="B71" s="5"/>
-      <c r="C71" s="5">
-        <v>0.75</v>
-      </c>
-      <c r="D71" s="5"/>
-      <c r="E71">
-        <f>A73-C73</f>
-        <v>0.23314500000000005</v>
-      </c>
-      <c r="F71">
-        <f>A67-F69</f>
-        <v>5111.9199999999983</v>
-      </c>
-      <c r="G71" s="5"/>
-      <c r="H71" s="5">
-        <f>SUM(J6,J9,J13,J17)/14*1000000</f>
-        <v>416.33035714285717</v>
-      </c>
-      <c r="I71" s="5"/>
-      <c r="J71" s="5"/>
-      <c r="K71" s="5"/>
-      <c r="L71" s="9"/>
-    </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A72" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="B72" s="5"/>
-      <c r="C72" t="s">
+      <c r="AF69" s="5"/>
+      <c r="AG69" s="5"/>
+      <c r="AH69" s="5"/>
+      <c r="AI69" s="9"/>
+    </row>
+    <row r="70" spans="24:35" x14ac:dyDescent="0.4">
+      <c r="Y70" s="5"/>
+      <c r="Z70" s="5">
+        <v>0.8</v>
+      </c>
+      <c r="AA70" s="5"/>
+      <c r="AB70">
+        <f>X72-Z72</f>
+        <v>0.12689459999999997</v>
+      </c>
+      <c r="AC70">
+        <f>X66-AC68</f>
+        <v>9545.9520000000048</v>
+      </c>
+      <c r="AD70" s="5"/>
+      <c r="AE70" s="5">
+        <f>SUM(J4,J7,J10,J14)/14*1000000</f>
+        <v>59.488000000000007</v>
+      </c>
+      <c r="AF70" s="5"/>
+      <c r="AG70" s="5"/>
+      <c r="AH70" s="5"/>
+      <c r="AI70" s="9"/>
+    </row>
+    <row r="71" spans="24:35" x14ac:dyDescent="0.4">
+      <c r="X71" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="Y71" s="5"/>
+      <c r="Z71" t="s">
         <v>39</v>
       </c>
-      <c r="D72" s="5"/>
-      <c r="E72" s="5" t="s">
+      <c r="AA71" s="5"/>
+      <c r="AB71" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="F72" s="5"/>
-      <c r="G72" s="5"/>
-      <c r="H72" s="5" t="s">
+      <c r="AC71" s="5"/>
+      <c r="AD71" s="5"/>
+      <c r="AE71" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="I72" s="5"/>
-      <c r="J72" s="5"/>
-      <c r="K72" s="5"/>
-      <c r="L72" s="9"/>
-    </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A73" s="4">
-        <f>A70/5*4.5</f>
-        <v>0.93258000000000008</v>
-      </c>
-      <c r="C73">
-        <f>A73*C71</f>
-        <v>0.69943500000000003</v>
-      </c>
-      <c r="E73">
-        <f>F71/A76</f>
-        <v>338247.7602045401</v>
-      </c>
-      <c r="H73">
-        <f>H67-H71</f>
-        <v>27.755357142857122</v>
-      </c>
-      <c r="L73" s="9"/>
-    </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A74" s="5"/>
-      <c r="B74" s="5"/>
-      <c r="C74" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="D74" s="5"/>
-      <c r="E74" s="5"/>
-      <c r="F74" s="5"/>
-      <c r="G74" s="5"/>
-      <c r="H74" s="5" t="s">
+      <c r="AF71" s="5"/>
+      <c r="AG71" s="5"/>
+      <c r="AH71" s="5"/>
+      <c r="AI71" s="9"/>
+    </row>
+    <row r="72" spans="24:35" x14ac:dyDescent="0.4">
+      <c r="X72" s="4">
+        <f>X75*Z75</f>
+        <v>0.63447299999999995</v>
+      </c>
+      <c r="Z72">
+        <f>X72*Z70</f>
+        <v>0.50757839999999999</v>
+      </c>
+      <c r="AB72">
+        <f>AC70/X75</f>
+        <v>947865.35597259505</v>
+      </c>
+      <c r="AE72">
+        <f>AE66-AE70</f>
+        <v>1469.7919999999999</v>
+      </c>
+      <c r="AI72" s="9"/>
+    </row>
+    <row r="73" spans="24:35" x14ac:dyDescent="0.4">
+      <c r="X73" s="5"/>
+      <c r="Y73" s="5"/>
+      <c r="Z73" s="5"/>
+      <c r="AA73" s="5"/>
+      <c r="AB73" s="5"/>
+      <c r="AC73" s="5"/>
+      <c r="AD73" s="5"/>
+      <c r="AE73" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="I74" s="5"/>
-      <c r="J74" s="5"/>
-      <c r="K74" s="5"/>
-      <c r="L74" s="9"/>
-    </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A75" s="14" t="s">
-        <v>50</v>
-      </c>
-      <c r="B75" s="5"/>
-      <c r="C75" s="5">
-        <f>C73/A76</f>
-        <v>46.280521244202298</v>
-      </c>
-      <c r="D75" s="5"/>
-      <c r="E75" s="5"/>
-      <c r="F75" s="5"/>
-      <c r="G75" s="5"/>
-      <c r="H75" s="5">
-        <f>H73/A76</f>
-        <v>1836.5286208016771</v>
-      </c>
-      <c r="I75" s="5"/>
-      <c r="J75" s="5"/>
-      <c r="K75" s="5"/>
-      <c r="L75" s="9"/>
-    </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A76" s="14">
-        <f>SUM(N6,N9,N13,N17)</f>
-        <v>1.5112945602090002E-2</v>
-      </c>
-      <c r="B76" s="5"/>
-      <c r="C76" s="5"/>
-      <c r="D76" s="5"/>
-      <c r="E76" s="5"/>
-      <c r="F76" s="5"/>
-      <c r="G76" s="5"/>
-      <c r="H76" s="5"/>
-      <c r="I76" s="5"/>
-      <c r="J76" s="5"/>
-      <c r="K76" s="5"/>
-      <c r="L76" s="9"/>
-    </row>
-    <row r="77" spans="1:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A77" s="11"/>
-      <c r="B77" s="11"/>
-      <c r="C77" s="11"/>
-      <c r="D77" s="11"/>
-      <c r="E77" s="11"/>
-      <c r="F77" s="11"/>
-      <c r="G77" s="11"/>
-      <c r="H77" s="11"/>
-      <c r="I77" s="11"/>
-      <c r="J77" s="11"/>
-      <c r="K77" s="11"/>
-      <c r="L77" s="12"/>
+      <c r="AF73" s="5"/>
+      <c r="AG73" s="5"/>
+      <c r="AH73" s="5"/>
+      <c r="AI73" s="9"/>
+    </row>
+    <row r="74" spans="24:35" x14ac:dyDescent="0.4">
+      <c r="X74" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="Y74" s="5"/>
+      <c r="Z74" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="AA74" s="5"/>
+      <c r="AB74" s="5"/>
+      <c r="AC74" s="5"/>
+      <c r="AD74" s="5"/>
+      <c r="AE74" s="5">
+        <f>AE72/X75</f>
+        <v>145943.00466686525</v>
+      </c>
+      <c r="AF74" s="5"/>
+      <c r="AG74" s="5"/>
+      <c r="AH74" s="5"/>
+      <c r="AI74" s="9"/>
+    </row>
+    <row r="75" spans="24:35" x14ac:dyDescent="0.4">
+      <c r="X75" s="14">
+        <f>SUM(N4,N7,N10,N14)</f>
+        <v>1.0071E-2</v>
+      </c>
+      <c r="Y75" s="5"/>
+      <c r="Z75" s="3">
+        <v>63</v>
+      </c>
+      <c r="AA75" s="5"/>
+      <c r="AB75" s="5"/>
+      <c r="AC75" s="5"/>
+      <c r="AD75" s="5"/>
+      <c r="AE75" s="5"/>
+      <c r="AF75" s="5"/>
+      <c r="AG75" s="5"/>
+      <c r="AH75" s="5"/>
+      <c r="AI75" s="9"/>
+    </row>
+    <row r="76" spans="24:35" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="X76" s="11"/>
+      <c r="Y76" s="11"/>
+      <c r="Z76" s="11"/>
+      <c r="AA76" s="11"/>
+      <c r="AB76" s="11"/>
+      <c r="AC76" s="11"/>
+      <c r="AD76" s="11"/>
+      <c r="AE76" s="11"/>
+      <c r="AF76" s="11"/>
+      <c r="AG76" s="11"/>
+      <c r="AH76" s="11"/>
+      <c r="AI76" s="12"/>
     </row>
   </sheetData>
   <autoFilter ref="D1:D36"/>
   <phoneticPr fontId="18"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>